<commit_message>
forget password link apis and use of bodyparser and use of ejs
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>S.no</t>
   </si>
@@ -92,6 +92,18 @@
   </si>
   <si>
     <t>ndehkgfgfsa</t>
+  </si>
+  <si>
+    <t>Jim Hadid</t>
+  </si>
+  <si>
+    <t>jherkhdbg121@gmail.com</t>
+  </si>
+  <si>
+    <t>Hemma Hadid</t>
+  </si>
+  <si>
+    <t>jhfrgeywuhdsj121@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -472,7 +484,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E13"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -641,6 +653,34 @@
         <v>26</v>
       </c>
     </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12">
+        <v>9226475786</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13">
+        <v>9226461104</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>